<commit_message>
Updated ExcelUtils to fetch login credentials and optimised DataProviderUtils
</commit_message>
<xml_diff>
--- a/completeseleniumproj/src/test/resources/excel/testdata.xlsx
+++ b/completeseleniumproj/src/test/resources/excel/testdata.xlsx
@@ -7,13 +7,13 @@
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
     <sheet name="RUNMANAGER" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet 1" sheetId="3" r:id="rId6"/>
+    <sheet name="DATA" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -37,7 +37,7 @@
       <rPr>
         <u val="single"/>
         <sz val="12"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>RUNMANAGER</t>
@@ -51,7 +51,7 @@
       <rPr>
         <u val="single"/>
         <sz val="12"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>Sheet 1</t>
@@ -91,9 +91,6 @@
     <t>To check if this test is executed</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -106,31 +103,31 @@
     <t>firstname</t>
   </si>
   <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>1234</t>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
   <si>
     <t>vishwa</t>
   </si>
   <si>
-    <t>shindhe</t>
-  </si>
-  <si>
-    <t>efgh</t>
-  </si>
-  <si>
-    <t>4567</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>qa</t>
+    <t>no</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>Admin123</t>
+  </si>
+  <si>
+    <t>test4</t>
   </si>
 </sst>
 </file>
@@ -164,7 +161,7 @@
     <font>
       <u val="single"/>
       <sz val="12"/>
-      <color indexed="12"/>
+      <color indexed="13"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
@@ -183,7 +180,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -195,13 +192,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="16"/>
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -212,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -222,11 +219,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -235,7 +232,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -243,17 +240,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
@@ -270,7 +267,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom/>
@@ -278,12 +275,12 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -292,160 +289,183 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="15"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="15"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="15"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
@@ -455,116 +475,131 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -584,6 +619,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
@@ -592,7 +628,6 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1779,7 +1814,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D10" location="'RUNMANAGER'!R1C1" tooltip="" display="RUNMANAGER"/>
-    <hyperlink ref="D12" location="'Sheet 1'!R1C1" tooltip="" display="Sheet 1"/>
+    <hyperlink ref="D12" location="'DATA'!R1C1" tooltip="" display="Sheet 1"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -1846,10 +1881,10 @@
         <v>19</v>
       </c>
       <c r="C3" t="s" s="27">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s" s="27">
         <v>20</v>
-      </c>
-      <c r="D3" t="s" s="27">
-        <v>21</v>
       </c>
       <c r="E3" t="s" s="27">
         <v>17</v>
@@ -1915,253 +1950,231 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="31" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="31" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="31" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="32">
-        <v>5</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
+    <row r="1" ht="20.25" customHeight="1">
+      <c r="A1" t="s" s="21">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s" s="21">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s" s="21">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s" s="21">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s" s="21">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="21">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s" s="21">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s" s="21">
+      <c r="A2" t="s" s="32">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s" s="33">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s" s="22">
         <v>24</v>
       </c>
-      <c r="D2" t="s" s="21">
+      <c r="D2" t="s" s="23">
         <v>25</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
+      <c r="E2" t="s" s="24">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
       <c r="A3" t="s" s="22">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s" s="23">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s" s="34">
         <v>27</v>
       </c>
-      <c r="C3" t="s" s="24">
+      <c r="C3" t="s" s="25">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s" s="35">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s" s="27">
         <v>28</v>
       </c>
-      <c r="D3" t="s" s="24">
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" t="s" s="36">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s" s="22">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s" s="37">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s" s="38">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s" s="27">
         <v>29</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="25">
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" t="s" s="39">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s" s="25">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s" s="37">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s" s="38">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s" s="27">
         <v>30</v>
       </c>
-      <c r="B4" t="s" s="26">
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" t="s" s="22">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s" s="40">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s" s="25">
         <v>31</v>
       </c>
-      <c r="C4" t="s" s="27">
+      <c r="D6" t="s" s="23">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s" s="27">
         <v>32</v>
       </c>
-      <c r="D4" t="s" s="27">
-        <v>33</v>
-      </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
       <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="29"/>
       <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="29"/>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="28"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="28"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="28"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="28"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
Adding support for Parallel Cross Browser Testing
</commit_message>
<xml_diff>
--- a/completeseleniumproj/src/test/resources/excel/testdata.xlsx
+++ b/completeseleniumproj/src/test/resources/excel/testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -94,6 +94,9 @@
     <t>2</t>
   </si>
   <si>
+    <t>browser</t>
+  </si>
+  <si>
     <t>username</t>
   </si>
   <si>
@@ -101,6 +104,9 @@
   </si>
   <si>
     <t>firstname</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
   <si>
     <t>Admin</t>
@@ -581,10 +587,10 @@
     <xf numFmtId="49" fontId="5" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="6" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1950,14 +1956,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="31" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="31" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="31" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1976,6 +1982,9 @@
       <c r="E1" t="s" s="21">
         <v>23</v>
       </c>
+      <c r="F1" t="s" s="21">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="32">
@@ -1984,14 +1993,17 @@
       <c r="B2" t="s" s="33">
         <v>16</v>
       </c>
-      <c r="C2" t="s" s="22">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s" s="23">
+      <c r="C2" t="s" s="33">
         <v>25</v>
       </c>
-      <c r="E2" t="s" s="24">
+      <c r="D2" t="s" s="22">
         <v>26</v>
+      </c>
+      <c r="E2" t="s" s="23">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s" s="24">
+        <v>28</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
@@ -1999,33 +2011,39 @@
         <v>14</v>
       </c>
       <c r="B3" t="s" s="34">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s" s="35">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s" s="25">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s" s="36">
         <v>27</v>
       </c>
-      <c r="C3" t="s" s="25">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s" s="35">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s" s="27">
-        <v>28</v>
+      <c r="F3" t="s" s="27">
+        <v>30</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="36">
+      <c r="A4" t="s" s="35">
         <v>18</v>
       </c>
       <c r="B4" t="s" s="22">
         <v>16</v>
       </c>
       <c r="C4" t="s" s="37">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s" s="38">
         <v>25</v>
       </c>
-      <c r="E4" t="s" s="27">
-        <v>29</v>
+      <c r="D4" t="s" s="37">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s" s="38">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s" s="27">
+        <v>31</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
@@ -2033,16 +2051,19 @@
         <v>18</v>
       </c>
       <c r="B5" t="s" s="25">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s" s="37">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s" s="37">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s" s="38">
         <v>27</v>
       </c>
-      <c r="C5" t="s" s="37">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s" s="38">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s" s="27">
-        <v>30</v>
+      <c r="F5" t="s" s="27">
+        <v>32</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
@@ -2052,127 +2073,146 @@
       <c r="B6" t="s" s="40">
         <v>16</v>
       </c>
-      <c r="C6" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s" s="23">
+      <c r="C6" t="s" s="35">
         <v>25</v>
       </c>
-      <c r="E6" t="s" s="27">
-        <v>32</v>
+      <c r="D6" t="s" s="25">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s" s="23">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s" s="27">
+        <v>34</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" s="41"/>
       <c r="B7" s="41"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" s="41"/>
       <c r="B8" s="41"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" s="41"/>
       <c r="B9" s="41"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" s="41"/>
       <c r="B10" s="41"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" s="41"/>
       <c r="B11" s="41"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="30"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" s="41"/>
       <c r="B12" s="41"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="30"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" s="41"/>
       <c r="B13" s="41"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="30"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" s="41"/>
       <c r="B14" s="41"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" s="41"/>
       <c r="B15" s="41"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" s="41"/>
       <c r="B16" s="41"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" s="41"/>
       <c r="B17" s="41"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="30"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" s="41"/>
       <c r="B18" s="41"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="30"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" s="41"/>
       <c r="B19" s="41"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="30"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" s="41"/>
       <c r="B20" s="41"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="30"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" s="41"/>
       <c r="B21" s="41"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="30"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" s="41"/>
       <c r="B22" s="41"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="30"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>

<commit_message>
Adding Amazon test and password encoding
</commit_message>
<xml_diff>
--- a/completeseleniumproj/src/test/resources/excel/testdata.xlsx
+++ b/completeseleniumproj/src/test/resources/excel/testdata.xlsx
@@ -5,9 +5,8 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
-    <sheet name="RUNMANAGER" sheetId="2" r:id="rId5"/>
-    <sheet name="DATA" sheetId="3" r:id="rId6"/>
+    <sheet name="RUNMANAGER" sheetId="1" r:id="rId4"/>
+    <sheet name="DATA" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -15,49 +14,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
-    <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
-  </si>
-  <si>
-    <t>Numbers Sheet Name</t>
-  </si>
-  <si>
-    <t>Numbers Table Name</t>
-  </si>
-  <si>
-    <t>Excel Worksheet Name</t>
-  </si>
-  <si>
-    <t>RUNMANAGER</t>
-  </si>
-  <si>
-    <t>Table 1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="12"/>
-        <color indexed="13"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>RUNMANAGER</t>
-    </r>
-  </si>
-  <si>
-    <t>Sheet 1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="12"/>
-        <color indexed="13"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>Sheet 1</t>
-    </r>
-  </si>
-  <si>
     <t>testname</t>
   </si>
   <si>
@@ -76,7 +32,7 @@
     <t>loginLogoutTest</t>
   </si>
   <si>
-    <t>To check whether user can successfully login and logout</t>
+    <t xml:space="preserve">To check whether the user can successfully login and logout </t>
   </si>
   <si>
     <t>yes</t>
@@ -88,52 +44,79 @@
     <t>newTest</t>
   </si>
   <si>
-    <t>To check if this test is executed</t>
+    <t xml:space="preserve">To check whether this test is executed </t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
+    <t>amazonTest</t>
+  </si>
+  <si>
+    <t>To check whether the amazon test is working or not</t>
+  </si>
+  <si>
     <t>browser</t>
   </si>
   <si>
+    <t>version</t>
+  </si>
+  <si>
     <t>username</t>
   </si>
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>firstname</t>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>menutext</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>88.0.4324.96</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>YWRtaW4xMjM=</t>
+  </si>
+  <si>
+    <t>amuthan</t>
   </si>
   <si>
     <t>firefox</t>
   </si>
   <si>
-    <t>Admin</t>
+    <t>69.0</t>
+  </si>
+  <si>
+    <t>testing mini bytes</t>
+  </si>
+  <si>
+    <t>79.0.3945.117</t>
   </si>
   <si>
     <t>admin123</t>
   </si>
   <si>
-    <t>vishwa</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>Admin123</t>
-  </si>
-  <si>
-    <t>test4</t>
+    <t>subscribe</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>124.0.2</t>
+  </si>
+  <si>
+    <t>Laptops</t>
   </si>
 </sst>
 </file>
@@ -143,11 +126,11 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12"/>
@@ -160,24 +143,12 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="22"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <color indexed="13"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,37 +161,28 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="14"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="21">
+  <borders count="8">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -260,31 +222,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -310,303 +247,48 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="16"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="16"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="16"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,22 +309,15 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff5e88b1"/>
-      <rgbColor rgb="ffeef3f4"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Blank">
+    <a:clrScheme name="Office Theme">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
@@ -656,22 +331,22 @@
         <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="00A2FF"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="16E7CF"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="61D836"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFD932"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF644E"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="FF42A1"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -680,7 +355,7 @@
         <a:srgbClr val="FF00FF"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Blank">
+    <a:fontScheme name="Office Theme">
       <a:majorFont>
         <a:latin typeface="Helvetica Neue"/>
         <a:ea typeface="Helvetica Neue"/>
@@ -692,7 +367,7 @@
         <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Blank">
+    <a:fmtScheme name="Office Theme">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -765,13 +440,31 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -839,10 +532,16 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1128,7 +827,13 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1413,7 +1118,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1695,134 +1400,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="4" width="33.6719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.8516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="101.172" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1719" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.7" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" ht="14.7" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" ht="8" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" t="s" s="8">
+    <row r="1" ht="28.8" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" ht="14.7" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" ht="14.7" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" ht="14.7" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" ht="18.6" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" t="s" s="9">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="9">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="9">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" ht="14.7" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" ht="16.65" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" t="s" s="10">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" ht="16.65" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="12"/>
-      <c r="C10" t="s" s="13">
+    </row>
+    <row r="2" ht="28.8" customHeight="1">
+      <c r="A2" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="14">
+      <c r="B2" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" ht="16.65" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" t="s" s="10">
+      <c r="C2" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" ht="16.65" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" t="s" s="17">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s" s="18">
+      <c r="D2" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="E12" s="19"/>
+      <c r="E2" t="s" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" ht="28.8" customHeight="1">
+      <c r="A3" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" ht="28.8" customHeight="1">
+      <c r="A4" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:D3"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D10" location="'RUNMANAGER'!R1C1" tooltip="" display="RUNMANAGER"/>
-    <hyperlink ref="D12" location="'DATA'!R1C1" tooltip="" display="Sheet 1"/>
-  </hyperlinks>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
@@ -1832,393 +1535,219 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="20" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="20" customWidth="1"/>
+    <col min="1" max="1" width="30.1719" style="4" customWidth="1"/>
+    <col min="2" max="3" width="18.1719" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.6719" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.6719" style="4" customWidth="1"/>
+    <col min="6" max="6" width="29.8516" style="4" customWidth="1"/>
+    <col min="7" max="7" width="30.8516" style="4" customWidth="1"/>
+    <col min="8" max="8" width="17.1719" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="8.85156" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="21">
+    <row r="1" ht="28.8" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" ht="28.8" customHeight="1">
+      <c r="A2" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" ht="28.8" customHeight="1">
+      <c r="A3" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" ht="28.8" customHeight="1">
+      <c r="A4" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="B1" t="s" s="21">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s" s="21">
+      <c r="B4" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="D1" t="s" s="21">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s" s="21">
+      <c r="C4" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" ht="28.8" customHeight="1">
+      <c r="A5" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" ht="28.8" customHeight="1">
+      <c r="A6" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" ht="34.05" customHeight="1">
+      <c r="A7" t="s" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" ht="50.25" customHeight="1">
-      <c r="A2" t="s" s="22">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s" s="23">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s" s="24">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s" s="24">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s" s="24">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" ht="26.05" customHeight="1">
-      <c r="A3" t="s" s="25">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s" s="26">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s" s="27">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s" s="27">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s" s="27">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" ht="14.05" customHeight="1">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-    </row>
-    <row r="5" ht="14.05" customHeight="1">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-    </row>
-    <row r="6" ht="14.05" customHeight="1">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-    </row>
-    <row r="7" ht="14.05" customHeight="1">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-    </row>
-    <row r="8" ht="14.05" customHeight="1">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-    </row>
-    <row r="9" ht="14.05" customHeight="1">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-    </row>
-    <row r="10" ht="14.05" customHeight="1">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
+      <c r="B7" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" t="s" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="6" width="16.3516" style="31" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="31" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" t="s" s="21">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s" s="21">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s" s="21">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s" s="21">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s" s="21">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s" s="21">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="32">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s" s="33">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s" s="33">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s" s="22">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s" s="23">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s" s="24">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="22">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s" s="34">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s" s="35">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s" s="25">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s" s="36">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s" s="27">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="35">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s" s="22">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s" s="37">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s" s="37">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s" s="38">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s" s="27">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="39">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s" s="25">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s" s="37">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s" s="37">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s" s="38">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s" s="27">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="22">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s" s="40">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s" s="35">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s" s="25">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s" s="23">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s" s="27">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="41"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="30"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="30"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="30"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="30"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="30"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="30"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="30"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>